<commit_message>
Added runs with prop bouncing
</commit_message>
<xml_diff>
--- a/linearization_heuristic_dyn_models/linearization_heuristic_results.xlsx
+++ b/linearization_heuristic_dyn_models/linearization_heuristic_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
   <si>
     <t>heuristic</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>linearization_heuristic</t>
+  </si>
+  <si>
+    <t>linearization_heuristic_Prop_Bouncing</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,25 +450,25 @@
         <v>0.5</v>
       </c>
       <c r="D2">
+        <v>37199.03</v>
+      </c>
+      <c r="E2">
+        <v>2000</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
-      <c r="E2">
-        <v>2500</v>
-      </c>
-      <c r="F2">
-        <v>30000</v>
-      </c>
       <c r="G2" t="s">
         <v>9</v>
       </c>
       <c r="H2">
-        <v>9902479187.045532</v>
+        <v>45126219367.12358</v>
       </c>
       <c r="I2">
-        <v>24098.35838258568</v>
+        <v>57171.15886280874</v>
       </c>
       <c r="J2">
-        <v>7721994539.664077</v>
+        <v>36715096117.55436</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -473,31 +476,479 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>0.5</v>
       </c>
       <c r="D3">
-        <v>1e+16</v>
+        <v>37199.03</v>
       </c>
       <c r="E3">
+        <v>2000</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>45118078147.20823</v>
+      </c>
+      <c r="I3">
+        <v>57699.84257550366</v>
+      </c>
+      <c r="J3">
+        <v>35290562905.46992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>37199.03</v>
+      </c>
+      <c r="E4">
+        <v>2000</v>
+      </c>
+      <c r="F4">
+        <v>30000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>45131647117.24555</v>
+      </c>
+      <c r="I4">
+        <v>57107.24397790962</v>
+      </c>
+      <c r="J4">
+        <v>36736088489.44138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>37199.03</v>
+      </c>
+      <c r="E5">
+        <v>2000</v>
+      </c>
+      <c r="F5">
+        <v>30000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>45123749290.05727</v>
+      </c>
+      <c r="I5">
+        <v>57624.94977265179</v>
+      </c>
+      <c r="J5">
+        <v>35292888524.85515</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>37199.03</v>
+      </c>
+      <c r="E6">
         <v>2500</v>
       </c>
-      <c r="F3">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>45131516387.95518</v>
+      </c>
+      <c r="I6">
+        <v>54747.01917833885</v>
+      </c>
+      <c r="J6">
+        <v>38282778527.67229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>37199.03</v>
+      </c>
+      <c r="E7">
+        <v>2500</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>45121956421.80877</v>
+      </c>
+      <c r="I7">
+        <v>55519.77062558438</v>
+      </c>
+      <c r="J7">
+        <v>35679091948.48907</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>37199.03</v>
+      </c>
+      <c r="E8">
+        <v>2500</v>
+      </c>
+      <c r="F8">
         <v>30000</v>
       </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>6367967226.456247</v>
-      </c>
-      <c r="I3">
-        <v>20964.25078365137</v>
-      </c>
-      <c r="J3">
-        <v>-2.096425078321849e+20</v>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>45134821358.37608</v>
+      </c>
+      <c r="I8">
+        <v>54690.63204528525</v>
+      </c>
+      <c r="J8">
+        <v>38288231012.26033</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>37199.03</v>
+      </c>
+      <c r="E9">
+        <v>2500</v>
+      </c>
+      <c r="F9">
+        <v>30000</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>45125616813.03027</v>
+      </c>
+      <c r="I9">
+        <v>55432.6300721997</v>
+      </c>
+      <c r="J9">
+        <v>35681435631.15625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>1115970.9</v>
+      </c>
+      <c r="E10">
+        <v>2000</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>38378161971.00523</v>
+      </c>
+      <c r="I10">
+        <v>53315.87091570689</v>
+      </c>
+      <c r="J10">
+        <v>-27092402351.21523</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>1115970.9</v>
+      </c>
+      <c r="E11">
+        <v>2000</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>38368879206.55049</v>
+      </c>
+      <c r="I11">
+        <v>53798.68238770959</v>
+      </c>
+      <c r="J11">
+        <v>-28744215536.2496</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>1115970.9</v>
+      </c>
+      <c r="E12">
+        <v>2000</v>
+      </c>
+      <c r="F12">
+        <v>30000</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>38787866014.70913</v>
+      </c>
+      <c r="I12">
+        <v>53183.7696675407</v>
+      </c>
+      <c r="J12">
+        <v>-26545854465.35203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <v>1115970.9</v>
+      </c>
+      <c r="E13">
+        <v>2000</v>
+      </c>
+      <c r="F13">
+        <v>30000</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>38778871591.62547</v>
+      </c>
+      <c r="I13">
+        <v>53669.29678369571</v>
+      </c>
+      <c r="J13">
+        <v>-28224255339.21764</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14">
+        <v>1115970.9</v>
+      </c>
+      <c r="E14">
+        <v>2500</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14">
+        <v>38368666066.33988</v>
+      </c>
+      <c r="I14">
+        <v>50692.80264486479</v>
+      </c>
+      <c r="J14">
+        <v>-22373676013.77703</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>0.5</v>
+      </c>
+      <c r="D15">
+        <v>1115970.9</v>
+      </c>
+      <c r="E15">
+        <v>2500</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <v>38357537429.8532</v>
+      </c>
+      <c r="I15">
+        <v>51552.28436569664</v>
+      </c>
+      <c r="J15">
+        <v>-25926212268.6306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+      <c r="D16">
+        <v>1115970.9</v>
+      </c>
+      <c r="E16">
+        <v>2500</v>
+      </c>
+      <c r="F16">
+        <v>30000</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16">
+        <v>38698847488.28083</v>
+      </c>
+      <c r="I16">
+        <v>50511.52088501569</v>
+      </c>
+      <c r="J16">
+        <v>-21869716022.38104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="D17">
+        <v>1115970.9</v>
+      </c>
+      <c r="E17">
+        <v>2500</v>
+      </c>
+      <c r="F17">
+        <v>30000</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <v>38688269129.18291</v>
+      </c>
+      <c r="I17">
+        <v>51369.997967439</v>
+      </c>
+      <c r="J17">
+        <v>-25413388073.41135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected bug in profilin-lin heur.
</commit_message>
<xml_diff>
--- a/linearization_heuristic_dyn_models/linearization_heuristic_results.xlsx
+++ b/linearization_heuristic_dyn_models/linearization_heuristic_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>heuristic</t>
   </si>
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,10 +450,10 @@
         <v>0.5</v>
       </c>
       <c r="D2">
-        <v>37199.03</v>
+        <v>3719903</v>
       </c>
       <c r="E2">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -462,13 +462,13 @@
         <v>9</v>
       </c>
       <c r="H2">
-        <v>45126219367.12358</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>57171.15886280874</v>
+        <v>15010.09194580075</v>
       </c>
       <c r="J2">
-        <v>36715096117.55436</v>
+        <v>-56644092239.61348</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -482,10 +482,10 @@
         <v>0.5</v>
       </c>
       <c r="D3">
-        <v>37199.03</v>
+        <v>3719903</v>
       </c>
       <c r="E3">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -494,13 +494,13 @@
         <v>9</v>
       </c>
       <c r="H3">
-        <v>45118078147.20823</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>57699.84257550366</v>
+        <v>15365.0777104941</v>
       </c>
       <c r="J3">
-        <v>35290562905.46992</v>
+        <v>-59290533449.26997</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -514,10 +514,10 @@
         <v>0.5</v>
       </c>
       <c r="D4">
-        <v>37199.03</v>
+        <v>3719903</v>
       </c>
       <c r="E4">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="F4">
         <v>30000</v>
@@ -526,13 +526,13 @@
         <v>9</v>
       </c>
       <c r="H4">
-        <v>45131647117.24555</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>57107.24397790962</v>
+        <v>14776.40162123898</v>
       </c>
       <c r="J4">
-        <v>36736088489.44138</v>
+        <v>-55761164228.44244</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -546,10 +546,10 @@
         <v>0.5</v>
       </c>
       <c r="D5">
-        <v>37199.03</v>
+        <v>3719903</v>
       </c>
       <c r="E5">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="F5">
         <v>30000</v>
@@ -558,397 +558,13 @@
         <v>9</v>
       </c>
       <c r="H5">
-        <v>45123749290.05727</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>57624.94977265179</v>
+        <v>15131.02357832273</v>
       </c>
       <c r="J5">
-        <v>35292888524.85515</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>0.5</v>
-      </c>
-      <c r="D6">
-        <v>37199.03</v>
-      </c>
-      <c r="E6">
-        <v>2500</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>45131516387.95518</v>
-      </c>
-      <c r="I6">
-        <v>54747.01917833885</v>
-      </c>
-      <c r="J6">
-        <v>38282778527.67229</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>0.5</v>
-      </c>
-      <c r="D7">
-        <v>37199.03</v>
-      </c>
-      <c r="E7">
-        <v>2500</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7">
-        <v>45121956421.80877</v>
-      </c>
-      <c r="I7">
-        <v>55519.77062558438</v>
-      </c>
-      <c r="J7">
-        <v>35679091948.48907</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>0.5</v>
-      </c>
-      <c r="D8">
-        <v>37199.03</v>
-      </c>
-      <c r="E8">
-        <v>2500</v>
-      </c>
-      <c r="F8">
-        <v>30000</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8">
-        <v>45134821358.37608</v>
-      </c>
-      <c r="I8">
-        <v>54690.63204528525</v>
-      </c>
-      <c r="J8">
-        <v>38288231012.26033</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>0.5</v>
-      </c>
-      <c r="D9">
-        <v>37199.03</v>
-      </c>
-      <c r="E9">
-        <v>2500</v>
-      </c>
-      <c r="F9">
-        <v>30000</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9">
-        <v>45125616813.03027</v>
-      </c>
-      <c r="I9">
-        <v>55432.6300721997</v>
-      </c>
-      <c r="J9">
-        <v>35681435631.15625</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>0.5</v>
-      </c>
-      <c r="D10">
-        <v>1115970.9</v>
-      </c>
-      <c r="E10">
-        <v>2000</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10">
-        <v>38378161971.00523</v>
-      </c>
-      <c r="I10">
-        <v>53315.87091570689</v>
-      </c>
-      <c r="J10">
-        <v>-27092402351.21523</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>0.5</v>
-      </c>
-      <c r="D11">
-        <v>1115970.9</v>
-      </c>
-      <c r="E11">
-        <v>2000</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11">
-        <v>38368879206.55049</v>
-      </c>
-      <c r="I11">
-        <v>53798.68238770959</v>
-      </c>
-      <c r="J11">
-        <v>-28744215536.2496</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12">
-        <v>0.5</v>
-      </c>
-      <c r="D12">
-        <v>1115970.9</v>
-      </c>
-      <c r="E12">
-        <v>2000</v>
-      </c>
-      <c r="F12">
-        <v>30000</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12">
-        <v>38787866014.70913</v>
-      </c>
-      <c r="I12">
-        <v>53183.7696675407</v>
-      </c>
-      <c r="J12">
-        <v>-26545854465.35203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>0.5</v>
-      </c>
-      <c r="D13">
-        <v>1115970.9</v>
-      </c>
-      <c r="E13">
-        <v>2000</v>
-      </c>
-      <c r="F13">
-        <v>30000</v>
-      </c>
-      <c r="G13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13">
-        <v>38778871591.62547</v>
-      </c>
-      <c r="I13">
-        <v>53669.29678369571</v>
-      </c>
-      <c r="J13">
-        <v>-28224255339.21764</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14">
-        <v>0.5</v>
-      </c>
-      <c r="D14">
-        <v>1115970.9</v>
-      </c>
-      <c r="E14">
-        <v>2500</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14">
-        <v>38368666066.33988</v>
-      </c>
-      <c r="I14">
-        <v>50692.80264486479</v>
-      </c>
-      <c r="J14">
-        <v>-22373676013.77703</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15">
-        <v>0.5</v>
-      </c>
-      <c r="D15">
-        <v>1115970.9</v>
-      </c>
-      <c r="E15">
-        <v>2500</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15">
-        <v>38357537429.8532</v>
-      </c>
-      <c r="I15">
-        <v>51552.28436569664</v>
-      </c>
-      <c r="J15">
-        <v>-25926212268.6306</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16">
-        <v>0.5</v>
-      </c>
-      <c r="D16">
-        <v>1115970.9</v>
-      </c>
-      <c r="E16">
-        <v>2500</v>
-      </c>
-      <c r="F16">
-        <v>30000</v>
-      </c>
-      <c r="G16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16">
-        <v>38698847488.28083</v>
-      </c>
-      <c r="I16">
-        <v>50511.52088501569</v>
-      </c>
-      <c r="J16">
-        <v>-21869716022.38104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17">
-        <v>0.5</v>
-      </c>
-      <c r="D17">
-        <v>1115970.9</v>
-      </c>
-      <c r="E17">
-        <v>2500</v>
-      </c>
-      <c r="F17">
-        <v>30000</v>
-      </c>
-      <c r="G17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17">
-        <v>38688269129.18291</v>
-      </c>
-      <c r="I17">
-        <v>51369.997967439</v>
-      </c>
-      <c r="J17">
-        <v>-25413388073.41135</v>
+        <v>-58392391683.3102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished equivalente LP Model formulation.
</commit_message>
<xml_diff>
--- a/linearization_heuristic_dyn_models/linearization_heuristic_results.xlsx
+++ b/linearization_heuristic_dyn_models/linearization_heuristic_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>heuristic</t>
   </si>
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
         <v>0.5</v>
       </c>
       <c r="D2">
-        <v>3719903</v>
+        <v>1115970.9</v>
       </c>
       <c r="E2">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>11272651347.38185</v>
       </c>
       <c r="I2">
-        <v>15010.09194580075</v>
+        <v>18536.07700107334</v>
       </c>
       <c r="J2">
-        <v>-56644092239.61348</v>
+        <v>-11853029973.01902</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -482,89 +482,25 @@
         <v>0.5</v>
       </c>
       <c r="D3">
-        <v>3719903</v>
+        <v>1115970.9</v>
       </c>
       <c r="E3">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>11272146584.22761</v>
       </c>
       <c r="I3">
-        <v>15365.0777104941</v>
+        <v>18645.40180227152</v>
       </c>
       <c r="J3">
-        <v>-59290533449.26997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>0.5</v>
-      </c>
-      <c r="D4">
-        <v>3719903</v>
-      </c>
-      <c r="E4">
-        <v>2500</v>
-      </c>
-      <c r="F4">
-        <v>30000</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>14776.40162123898</v>
-      </c>
-      <c r="J4">
-        <v>-55761164228.44244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>0.5</v>
-      </c>
-      <c r="D5">
-        <v>3719903</v>
-      </c>
-      <c r="E5">
-        <v>2500</v>
-      </c>
-      <c r="F5">
-        <v>30000</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>15131.02357832273</v>
-      </c>
-      <c r="J5">
-        <v>-58392391683.3102</v>
+        <v>-12441723946.87802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>